<commit_message>
Created Routine frame, Button Handler Class, List Handler
</commit_message>
<xml_diff>
--- a/Database/StudentInfo.xlsx
+++ b/Database/StudentInfo.xlsx
@@ -18,45 +18,69 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="38">
   <si>
+    <t>UG02-32-13-001</t>
+  </si>
+  <si>
+    <t>CSE-400</t>
+  </si>
+  <si>
     <t>CSE-429</t>
   </si>
   <si>
     <t>CSE-441</t>
   </si>
   <si>
-    <t>CSE-400</t>
+    <t>UG02-32-13-004</t>
+  </si>
+  <si>
+    <t>UG02-32-13-005</t>
+  </si>
+  <si>
+    <t>UG02-32-13-006</t>
+  </si>
+  <si>
+    <t>UG02-32-13-009</t>
+  </si>
+  <si>
+    <t>UG02-32-13-012</t>
+  </si>
+  <si>
+    <t>CSE-309</t>
   </si>
   <si>
     <t>ECO-111</t>
   </si>
   <si>
-    <t>CSE-309</t>
-  </si>
-  <si>
-    <t>UG02-32-13-001</t>
-  </si>
-  <si>
-    <t>UG02-32-13-004</t>
-  </si>
-  <si>
-    <t>UG02-32-13-005</t>
-  </si>
-  <si>
-    <t>UG02-32-13-006</t>
-  </si>
-  <si>
-    <t>UG02-32-13-009</t>
-  </si>
-  <si>
-    <t>UG02-32-13-012</t>
-  </si>
-  <si>
     <t>UG02-32-13-013</t>
   </si>
   <si>
     <t>UG02-32-13-014</t>
   </si>
   <si>
+    <t>UG02-32-13-015</t>
+  </si>
+  <si>
+    <t>CSE-311</t>
+  </si>
+  <si>
+    <t>CSE-312</t>
+  </si>
+  <si>
+    <t>CSE-315</t>
+  </si>
+  <si>
+    <t>CSE-316</t>
+  </si>
+  <si>
+    <t>EEE-213</t>
+  </si>
+  <si>
+    <t>ENG-171</t>
+  </si>
+  <si>
+    <t>MATH-191</t>
+  </si>
+  <si>
     <t>UG02-32-13-020</t>
   </si>
   <si>
@@ -66,52 +90,28 @@
     <t>UG02-32-13-022</t>
   </si>
   <si>
-    <t>EEE-213</t>
+    <t>UG02-32-13-023</t>
+  </si>
+  <si>
+    <t>UG02-32-13-024</t>
+  </si>
+  <si>
+    <t>UG02-32-13-025</t>
   </si>
   <si>
     <t>MATH-195</t>
   </si>
   <si>
-    <t>CSE-311</t>
-  </si>
-  <si>
-    <t>CSE-312</t>
+    <t>UG02-32-13-027</t>
+  </si>
+  <si>
+    <t>CSE-307</t>
   </si>
   <si>
     <t>CSE-317</t>
   </si>
   <si>
     <t>CSE-318</t>
-  </si>
-  <si>
-    <t>CSE-315</t>
-  </si>
-  <si>
-    <t>CSE-316</t>
-  </si>
-  <si>
-    <t>CSE-307</t>
-  </si>
-  <si>
-    <t>MATH-191</t>
-  </si>
-  <si>
-    <t>UG02-32-13-015</t>
-  </si>
-  <si>
-    <t>ENG-171</t>
-  </si>
-  <si>
-    <t>UG02-32-13-023</t>
-  </si>
-  <si>
-    <t>UG02-32-13-024</t>
-  </si>
-  <si>
-    <t>UG02-32-13-025</t>
-  </si>
-  <si>
-    <t>UG02-32-13-027</t>
   </si>
   <si>
     <t>UG02-32-13-029</t>
@@ -463,175 +463,174 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
         <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -639,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -647,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -655,7 +654,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -663,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -671,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -679,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -687,247 +686,247 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
         <v>31</v>
-      </c>
-      <c r="B56" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -935,7 +934,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -943,7 +942,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -951,7 +950,7 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -959,7 +958,7 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -967,7 +966,7 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -975,7 +974,7 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -983,7 +982,7 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -991,7 +990,7 @@
         <v>33</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -999,7 +998,7 @@
         <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1007,7 +1006,7 @@
         <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1015,7 +1014,7 @@
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1023,7 +1022,7 @@
         <v>34</v>
       </c>
       <c r="B69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1031,7 +1030,7 @@
         <v>34</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1039,7 +1038,7 @@
         <v>35</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1047,7 +1046,7 @@
         <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1055,7 +1054,7 @@
         <v>35</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1063,7 +1062,7 @@
         <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1071,7 +1070,7 @@
         <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1079,7 +1078,7 @@
         <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1087,7 +1086,7 @@
         <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1095,7 +1094,7 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1103,7 +1102,7 @@
         <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1111,7 +1110,7 @@
         <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1119,7 +1118,7 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>